<commit_message>
Various changes. First, removed unnecessary references to URLs in jquery-ui.theme.min.css which were causing minute CSS errors. Added subtitles.css to style the subtitles and add opacity. Added new sleep function in helper.js for async/await. Modified videos-loaded-event.js to add a function that abstracts out something that users of videos-loaded-event.js will use often (but probably not a really good design choice, not too sure). modified init to include the new silence-cue-manager.js. Modified ts-tracker and audio worklet as well as silence cue-manager to implement silence detection. Modified speed-slider to 8 (most likely a temporary modification) to help test the buffering issue with the video players. Finally modified subtitles to sync the subs. More details on the subtitle fix in the issue.
</commit_message>
<xml_diff>
--- a/Skylab documents/Milestone 1 Submission/Submission 1/Project Log.xlsx
+++ b/Skylab documents/Milestone 1 Submission/Submission 1/Project Log.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Study\Y1 Summer\Panopto Project\Skylab documents\Milestone 1 Submission\Submission 1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF227836-D74B-4328-80DB-F6DE13FDE6A9}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9F204930-6306-4251-BCAA-A20B9E2A6F14}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="5480" xr2:uid="{18F59187-B1E2-45ED-BF88-DDFCC51EE406}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="36">
   <si>
     <t>Project Log</t>
   </si>
@@ -168,6 +168,21 @@
   <si>
     <t>1) Run through current state of project
 2) Crash course into HTML/CSS &amp; JS for Fyonn</t>
+  </si>
+  <si>
+    <t>1) Basic implementation of audio webworklet for FFT processing with window size of 512 samples.</t>
+  </si>
+  <si>
+    <t>1) Converted use of Promises to async/await for code clarity in webworklet &amp; subtitles.js
+2) Researched on TextTracks cues system
+3) Fixed subtitles bug involving Panopto's desynced two videos system (videos play at different offsets at different timings, only synced at runtime in implementation. Our implementation must thus also be synced at runtime)</t>
+  </si>
+  <si>
+    <t>1) Implemented silence detection using TextTracks oncuechange (cues system)
+2) Brainstorming for seeking videos (need to keep videos in sync)
+3) Discovered bug involving lag when seeking, bug appears to be involving buffering with HLSJS
+4) More research into Panopto's implementation, HLS.js documentation on their API, Debugging
+5) Implemented basic implementation of silence detection</t>
   </si>
 </sst>
 </file>
@@ -563,10 +578,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D66DA078-28E1-44A0-8117-A67A05B0BE09}">
-  <dimension ref="A1:F23"/>
+  <dimension ref="A1:F26"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="F22" sqref="F22"/>
+    <sheetView tabSelected="1" topLeftCell="A24" workbookViewId="0">
+      <selection activeCell="F25" sqref="F25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -931,28 +946,79 @@
         <v>32</v>
       </c>
     </row>
-    <row r="22" spans="2:6" x14ac:dyDescent="0.35">
-      <c r="C22" s="2" t="s">
+    <row r="22" spans="2:6" ht="29" x14ac:dyDescent="0.35">
+      <c r="B22" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="C22" s="9">
+        <v>43625</v>
+      </c>
+      <c r="D22" s="2">
+        <v>10</v>
+      </c>
+      <c r="E22" s="2">
+        <v>0</v>
+      </c>
+      <c r="F22" s="11" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="23" spans="2:6" ht="87" x14ac:dyDescent="0.35">
+      <c r="B23" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="C23" s="9">
+        <v>43626</v>
+      </c>
+      <c r="D23" s="2">
+        <v>6</v>
+      </c>
+      <c r="E23" s="2">
+        <v>0</v>
+      </c>
+      <c r="F23" s="11" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="24" spans="2:6" ht="116" x14ac:dyDescent="0.35">
+      <c r="B24" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="C24" s="9">
+        <v>43627</v>
+      </c>
+      <c r="D24" s="2">
+        <v>10</v>
+      </c>
+      <c r="E24" s="2">
+        <v>0</v>
+      </c>
+      <c r="F24" s="11" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="25" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="C25" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="D22" s="3" t="s">
+      <c r="D25" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="E22" s="3" t="s">
+      <c r="E25" s="3" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="23" spans="2:6" x14ac:dyDescent="0.35">
-      <c r="C23" s="1">
-        <f>SUM(D3:E20)</f>
-        <v>121</v>
-      </c>
-      <c r="D23" s="2">
-        <f>SUM(D3:D21)</f>
-        <v>118</v>
-      </c>
-      <c r="E23" s="2">
-        <f>SUM(E3:E21)</f>
+    <row r="26" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="C26" s="1">
+        <f>SUM(D26:E26)</f>
+        <v>159</v>
+      </c>
+      <c r="D26" s="2">
+        <f>SUM(D3:D24)</f>
+        <v>144</v>
+      </c>
+      <c r="E26" s="2">
+        <f>SUM(E3:E24)</f>
         <v>15</v>
       </c>
     </row>

</xml_diff>

<commit_message>
removed alert (subs) because it was interfering with texttrack initialization (it will remain as disabled of hidden). Revamped silence detection implementation significantly to use new method involving DCFT and noise samples as reference (see commments in vad-audio-worklet-processor.js for implementation details). However, distance threshold is variable. Thus, more work needs to be done to rectify that. Proposed solution is to implement an order statistic tree and get the 25th percentile of all the distances and use that as the threshold. This requires delaying of identification of speech and non-speech (in order to get sufficient data), thus moving code from TSTracker into a webworklet is also recommended.
</commit_message>
<xml_diff>
--- a/Skylab documents/Milestone 1 Submission/Submission 1/Project Log.xlsx
+++ b/Skylab documents/Milestone 1 Submission/Submission 1/Project Log.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Study\Y1 Summer\Panopto Project\Skylab documents\Milestone 1 Submission\Submission 1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9F204930-6306-4251-BCAA-A20B9E2A6F14}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D501D44-0CAD-42A8-B429-A0F8A7DB488D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="5480" xr2:uid="{18F59187-B1E2-45ED-BF88-DDFCC51EE406}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="37">
   <si>
     <t>Project Log</t>
   </si>
@@ -183,6 +183,9 @@
 3) Discovered bug involving lag when seeking, bug appears to be involving buffering with HLSJS
 4) More research into Panopto's implementation, HLS.js documentation on their API, Debugging
 5) Implemented basic implementation of silence detection</t>
+  </si>
+  <si>
+    <t>1) Voice Activity Detection research (https://www.ncbi.nlm.nih.gov/pmc/articles/PMC4142156/)</t>
   </si>
 </sst>
 </file>
@@ -578,10 +581,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D66DA078-28E1-44A0-8117-A67A05B0BE09}">
-  <dimension ref="A1:F26"/>
+  <dimension ref="A1:F27"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A24" workbookViewId="0">
-      <selection activeCell="F25" sqref="F25"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="F26" sqref="F26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -997,28 +1000,45 @@
         <v>35</v>
       </c>
     </row>
-    <row r="25" spans="2:6" x14ac:dyDescent="0.35">
-      <c r="C25" s="2" t="s">
+    <row r="25" spans="2:6" ht="29" x14ac:dyDescent="0.35">
+      <c r="B25" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="C25" s="9">
+        <v>43628</v>
+      </c>
+      <c r="D25" s="2">
+        <v>6</v>
+      </c>
+      <c r="E25" s="2">
+        <v>0</v>
+      </c>
+      <c r="F25" s="11" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="26" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="C26" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="D25" s="3" t="s">
+      <c r="D26" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="E25" s="3" t="s">
+      <c r="E26" s="3" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="26" spans="2:6" x14ac:dyDescent="0.35">
-      <c r="C26" s="1">
-        <f>SUM(D26:E26)</f>
-        <v>159</v>
-      </c>
-      <c r="D26" s="2">
-        <f>SUM(D3:D24)</f>
-        <v>144</v>
-      </c>
-      <c r="E26" s="2">
-        <f>SUM(E3:E24)</f>
+    <row r="27" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="C27" s="1">
+        <f>SUM(D27:E27)</f>
+        <v>165</v>
+      </c>
+      <c r="D27" s="2">
+        <f>SUM(D3:D25)</f>
+        <v>150</v>
+      </c>
+      <c r="E27" s="2">
+        <f>SUM(E3:E25)</f>
         <v>15</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Added a few new csv files for R analysis. Fixed context-bridge.js minor exec error. Added Order Statistic Tree for backup in case needed in the future. Modified ts-tracker, worklet and silence cue manager (see project log and files for change details). Removed the obsolete voice-detector.js file.
</commit_message>
<xml_diff>
--- a/Skylab documents/Milestone 1 Submission/Submission 1/Project Log.xlsx
+++ b/Skylab documents/Milestone 1 Submission/Submission 1/Project Log.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Study\Y1 Summer\Panopto Project\Skylab documents\Milestone 1 Submission\Submission 1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D501D44-0CAD-42A8-B429-A0F8A7DB488D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B2E95BB-C89E-4FE4-9FDD-E9085118E4A8}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="5480" xr2:uid="{18F59187-B1E2-45ED-BF88-DDFCC51EE406}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="40">
   <si>
     <t>Project Log</t>
   </si>
@@ -178,14 +178,32 @@
 3) Fixed subtitles bug involving Panopto's desynced two videos system (videos play at different offsets at different timings, only synced at runtime in implementation. Our implementation must thus also be synced at runtime)</t>
   </si>
   <si>
+    <t>1) Voice Activity Detection research (https://www.ncbi.nlm.nih.gov/pmc/articles/PMC4142156/)
+1.1) A TLDR on the paper: FFT to get magnitude of frequency bins, then FFT the magnitudes to get the "harmonic information in speech signals". Subsequently calculate the mean frequency bin index (Fmean) and the slope linear regression coefficients for both low index (0 to Fmean) and high index (Fmean to max). These calculated variables (Fmean and the coefficients) form the five-dimensional feature set that defines a "signal". So what it does is get the feature set of a slice of data that is assumed to be noise (which this app assumes to be the first 100ms). This feature set is defined as the reference feature. All subsequent feature sets are compared against this reference to test if they are "speech" or "noise". This comparison is done by taking the difference between each feature set and squashing it down to a single value (referred to as "distance" in the paper as well as in later parts of this project log)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1) Re-implementation of VAD based on paper (this sentence hides a lot of the implementation details involving DCFT and other optimizations, but it's basically what the paper describes in javascript, pre-calculated data and a few app-specific tweaks to minimize calculations); involved restructuring of ts-tracker &amp; vad-audio-worklet-processor for inter-thread communications.
+2) Completion of re-implementation and testing. Testing reveals that the noise - voice threshold (the distance value that determines if the signal at that point is "noise" or "voice") varies across different webcasts beyond what the paper has described. </t>
+  </si>
+  <si>
     <t>1) Implemented silence detection using TextTracks oncuechange (cues system)
 2) Brainstorming for seeking videos (need to keep videos in sync)
 3) Discovered bug involving lag when seeking, bug appears to be involving buffering with HLSJS
 4) More research into Panopto's implementation, HLS.js documentation on their API, Debugging
-5) Implemented basic implementation of silence detection</t>
-  </si>
-  <si>
-    <t>1) Voice Activity Detection research (https://www.ncbi.nlm.nih.gov/pmc/articles/PMC4142156/)</t>
+5) Implemented basic implementation of silence detection
+6) Potential of silence detection appears very promising. The webcast can be significantly shortened even mid-speech without impacting voice quality.</t>
+  </si>
+  <si>
+    <t>1) 1st attempt to dynamically obtain noise-voice threshold involves using an order statistic tree built on a Binary Indexed Tree (BIT) in order to get the value at the 25th percentile (or a similar method to avoid extreme outliers) and set that value as the threshold. Implementation deemed irrelevant after thought experiments reveal that the distribution of distances may be skewed towards speech / non-speech.
+2) Further thought experiments reveal that it may be more likely that the distribution of distances may follow a bimodal distribution (given that there's two states of "noise" and "no noise", and speech by a professor is likely to be restricted to a range of frequencies). 
+3) Checked this possibility by shifting the data out into a csv file and then plotting the histogram(s) of ~6 minutes long samples from multiple webcasts at different timings (x-axis: difference, y-axis: frequency of data occurance), as well as graphing distance against time using R. No conclusion can be made yet until more webcasts by different professors (and in different venues) have been sampled.
+4) Finished developmental work which allows for testing of thresholds</t>
+  </si>
+  <si>
+    <t>1) Observation shows that assumption that webcasts start with noise is unwarranted. Discovered some webcasts that start immediately with speech. Changed code to analyse the last TS file instead, and to only analyze the last section of the TS file. If the TS file is too short, use second last. Ignores last second of the webcast as the last second's video and presumably audio is faded out by Panopto.
+2) Program now retrieves 30 samples of noise as the reference sample and build mean &amp; std dev for each of the 5 variables. Using an arbitrary confidence level of 97.8% (based on some experimentation) for all variables, and majority of variables must exceed this confidence level for the signal to be defined as "non-noise". Seems to work well for all webcasts tested.
+3) Further analysis on how Panopto sync streams reveals clues on implementation. Desync issue (from jumping too much) resolved with a solution that combines efficiency &amp; desync resistance. 
+4) Added logger-disabler.js to disable logs produced by Panopto's code (to be fair, code in production shouldn't be producing logs...)</t>
   </si>
 </sst>
 </file>
@@ -581,10 +599,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D66DA078-28E1-44A0-8117-A67A05B0BE09}">
-  <dimension ref="A1:F27"/>
+  <dimension ref="A1:F33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="F26" sqref="F26"/>
+    <sheetView tabSelected="1" topLeftCell="A28" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="F29" sqref="F29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -983,7 +1001,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="24" spans="2:6" ht="116" x14ac:dyDescent="0.35">
+    <row r="24" spans="2:6" ht="145" x14ac:dyDescent="0.35">
       <c r="B24" s="10" t="s">
         <v>17</v>
       </c>
@@ -997,10 +1015,10 @@
         <v>0</v>
       </c>
       <c r="F24" s="11" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="25" spans="2:6" ht="29" x14ac:dyDescent="0.35">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="25" spans="2:6" ht="217.5" x14ac:dyDescent="0.35">
       <c r="B25" s="10" t="s">
         <v>17</v>
       </c>
@@ -1014,31 +1032,82 @@
         <v>0</v>
       </c>
       <c r="F25" s="11" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="26" spans="2:6" ht="130.5" x14ac:dyDescent="0.35">
+      <c r="B26" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="C26" s="9">
+        <v>43629</v>
+      </c>
+      <c r="D26" s="2">
+        <v>10</v>
+      </c>
+      <c r="E26" s="2">
+        <v>0</v>
+      </c>
+      <c r="F26" s="11" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="26" spans="2:6" x14ac:dyDescent="0.35">
-      <c r="C26" s="2" t="s">
+    <row r="27" spans="2:6" ht="246.5" x14ac:dyDescent="0.35">
+      <c r="B27" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="C27" s="9">
+        <v>43637</v>
+      </c>
+      <c r="D27" s="2">
+        <v>10</v>
+      </c>
+      <c r="E27" s="2">
+        <v>0</v>
+      </c>
+      <c r="F27" s="11" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="28" spans="2:6" ht="232" x14ac:dyDescent="0.35">
+      <c r="B28" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="C28" s="9">
+        <v>43638</v>
+      </c>
+      <c r="D28" s="2">
+        <v>10</v>
+      </c>
+      <c r="E28" s="2">
+        <v>0</v>
+      </c>
+      <c r="F28" s="11" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="32" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="C32" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="D26" s="3" t="s">
+      <c r="D32" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="E26" s="3" t="s">
+      <c r="E32" s="3" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="27" spans="2:6" x14ac:dyDescent="0.35">
-      <c r="C27" s="1">
-        <f>SUM(D27:E27)</f>
-        <v>165</v>
-      </c>
-      <c r="D27" s="2">
-        <f>SUM(D3:D25)</f>
-        <v>150</v>
-      </c>
-      <c r="E27" s="2">
-        <f>SUM(E3:E25)</f>
+    <row r="33" spans="3:5" x14ac:dyDescent="0.35">
+      <c r="C33" s="1">
+        <f>SUM(D33:E33)</f>
+        <v>195</v>
+      </c>
+      <c r="D33" s="2">
+        <f>SUM(D3:D32)</f>
+        <v>180</v>
+      </c>
+      <c r="E33" s="2">
+        <f>SUM(E3:E32)</f>
         <v>15</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Moved code to dev, added dist folder, more work on documentation
</commit_message>
<xml_diff>
--- a/Skylab documents/Milestone 1 Submission/Submission 1/Project Log.xlsx
+++ b/Skylab documents/Milestone 1 Submission/Submission 1/Project Log.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Study\Y1 Summer\Panopto Project\Skylab documents\Milestone 1 Submission\Submission 1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B2E95BB-C89E-4FE4-9FDD-E9085118E4A8}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D9B350E-036F-4F3A-A8D5-E1EC4ED1C9FC}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="5480" xr2:uid="{18F59187-B1E2-45ED-BF88-DDFCC51EE406}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="42">
   <si>
     <t>Project Log</t>
   </si>
@@ -204,6 +204,12 @@
 2) Program now retrieves 30 samples of noise as the reference sample and build mean &amp; std dev for each of the 5 variables. Using an arbitrary confidence level of 97.8% (based on some experimentation) for all variables, and majority of variables must exceed this confidence level for the signal to be defined as "non-noise". Seems to work well for all webcasts tested.
 3) Further analysis on how Panopto sync streams reveals clues on implementation. Desync issue (from jumping too much) resolved with a solution that combines efficiency &amp; desync resistance. 
 4) Added logger-disabler.js to disable logs produced by Panopto's code (to be fair, code in production shouldn't be producing logs...)</t>
+  </si>
+  <si>
+    <t>Documentation</t>
+  </si>
+  <si>
+    <t>1) Restructuring, removing irrelevant files, creating JSDocs &amp; documentation</t>
   </si>
 </sst>
 </file>
@@ -602,7 +608,7 @@
   <dimension ref="A1:F33"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A28" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="F29" sqref="F29"/>
+      <selection activeCell="F30" sqref="F30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1086,6 +1092,23 @@
         <v>39</v>
       </c>
     </row>
+    <row r="29" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B29" s="10" t="s">
+        <v>40</v>
+      </c>
+      <c r="C29" s="9">
+        <v>43639</v>
+      </c>
+      <c r="D29" s="2">
+        <v>5</v>
+      </c>
+      <c r="E29" s="2">
+        <v>0</v>
+      </c>
+      <c r="F29" s="11" t="s">
+        <v>41</v>
+      </c>
+    </row>
     <row r="32" spans="2:6" x14ac:dyDescent="0.35">
       <c r="C32" s="2" t="s">
         <v>15</v>
@@ -1100,11 +1123,11 @@
     <row r="33" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C33" s="1">
         <f>SUM(D33:E33)</f>
-        <v>195</v>
+        <v>200</v>
       </c>
       <c r="D33" s="2">
         <f>SUM(D3:D32)</f>
-        <v>180</v>
+        <v>185</v>
       </c>
       <c r="E33" s="2">
         <f>SUM(E3:E32)</f>

</xml_diff>